<commit_message>
maxZoom 4 -> 10
</commit_message>
<xml_diff>
--- a/레이어.xlsx
+++ b/레이어.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="18" uniqueCount="18">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
   <si>
     <t>레이어</t>
     <phoneticPr fontId="1" type="noConversion"/>
@@ -95,6 +95,14 @@
   </si>
   <si>
     <t>도면</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>조감도</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>지도</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -425,10 +433,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:D13"/>
+  <dimension ref="A1:D14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D7" sqref="D7"/>
+      <selection activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999" x14ac:dyDescent="0.4"/>
@@ -464,7 +472,10 @@
         <v>2</v>
       </c>
       <c r="C3" t="s">
-        <v>3</v>
+        <v>19</v>
+      </c>
+      <c r="D3" t="s">
+        <v>18</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.4">
@@ -472,7 +483,7 @@
         <v>3</v>
       </c>
       <c r="C4" t="s">
-        <v>4</v>
+        <v>3</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.4">
@@ -480,10 +491,7 @@
         <v>4</v>
       </c>
       <c r="C5" t="s">
-        <v>5</v>
-      </c>
-      <c r="D5" t="s">
-        <v>16</v>
+        <v>4</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.4">
@@ -491,7 +499,10 @@
         <v>5</v>
       </c>
       <c r="C6" t="s">
-        <v>6</v>
+        <v>5</v>
+      </c>
+      <c r="D6" t="s">
+        <v>16</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.4">
@@ -499,7 +510,7 @@
         <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>7</v>
+        <v>6</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.4">
@@ -507,7 +518,7 @@
         <v>7</v>
       </c>
       <c r="C8" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.4">
@@ -515,7 +526,7 @@
         <v>8</v>
       </c>
       <c r="C9" t="s">
-        <v>9</v>
+        <v>8</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.4">
@@ -523,10 +534,7 @@
         <v>9</v>
       </c>
       <c r="C10" t="s">
-        <v>10</v>
-      </c>
-      <c r="D10" t="s">
-        <v>17</v>
+        <v>9</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.4">
@@ -534,7 +542,10 @@
         <v>10</v>
       </c>
       <c r="C11" t="s">
-        <v>11</v>
+        <v>10</v>
+      </c>
+      <c r="D11" t="s">
+        <v>17</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.4">
@@ -542,7 +553,7 @@
         <v>11</v>
       </c>
       <c r="C12" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.4">
@@ -550,6 +561,14 @@
         <v>12</v>
       </c>
       <c r="C13" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.4">
+      <c r="A14">
+        <v>13</v>
+      </c>
+      <c r="C14" t="s">
         <v>13</v>
       </c>
     </row>

</xml_diff>